<commit_message>
Tile Type, Tier 설정
</commit_message>
<xml_diff>
--- a/Excel/EposTilePercent.xlsx
+++ b/Excel/EposTilePercent.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27109"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27123"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D2501A07-3137-4B08-B2E1-AE27ABF73D51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{6CE95D0A-941A-45CC-8812-9A0627AAB759}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,31 +36,31 @@
     <t>PlayerLevel</t>
   </si>
   <si>
-    <t>Level1Tile</t>
-  </si>
-  <si>
-    <t>Level2Tile</t>
-  </si>
-  <si>
-    <t>Level3Tile</t>
-  </si>
-  <si>
-    <t>Level4Tile</t>
-  </si>
-  <si>
-    <t>Level5Tile</t>
-  </si>
-  <si>
-    <t>Level6Tile</t>
-  </si>
-  <si>
-    <t>EmptyTile</t>
-  </si>
-  <si>
-    <t>UnmovableTile</t>
-  </si>
-  <si>
-    <t>ObjectTile</t>
+    <t>Tier1</t>
+  </si>
+  <si>
+    <t>Tier2</t>
+  </si>
+  <si>
+    <t>Tier3</t>
+  </si>
+  <si>
+    <t>Tier4</t>
+  </si>
+  <si>
+    <t>Tier5</t>
+  </si>
+  <si>
+    <t>Tier6</t>
+  </si>
+  <si>
+    <t>Empty</t>
+  </si>
+  <si>
+    <t>Unmovable</t>
+  </si>
+  <si>
+    <t>Object</t>
   </si>
 </sst>
 </file>
@@ -415,12 +415,12 @@
   <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
   <cols>
-    <col min="1" max="1" width="13.125" customWidth="1"/>
+    <col min="1" max="1" width="14.875" customWidth="1"/>
     <col min="9" max="9" width="13.375" customWidth="1"/>
     <col min="10" max="10" width="11.625" customWidth="1"/>
   </cols>

</xml_diff>